<commit_message>
Añadir documentos del TFM
</commit_message>
<xml_diff>
--- a/BBDD Tableau adicional.xlsx
+++ b/BBDD Tableau adicional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebep\OneDrive\Desktop\TFM\Anexos\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0610C2-2730-406A-8F01-1D9708410F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A7FF10-EDCD-4292-9ED5-AF3397F86EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="25">
   <si>
     <t>Timestamp</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Enfermedades digestivas</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -356,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -461,7 +464,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -918,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A3AC2E-D87F-45D8-A29F-A080CBA9C741}">
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -968,11 +970,13 @@
       <c r="A2" s="6">
         <v>45682.202848506946</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="52"/>
+      <c r="E2" s="51"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
@@ -987,11 +991,13 @@
       <c r="A3" s="27">
         <v>45673.927681203699</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="56"/>
+      <c r="E3" s="55"/>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
       <c r="H3" s="31"/>
@@ -1006,11 +1012,13 @@
       <c r="A4" s="6">
         <v>45672.398197604169</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="56"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="7"/>
@@ -1021,11 +1029,13 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>45656.715578784722</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1040,11 +1050,13 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>45666.934966377317</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1058,11 +1070,13 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="26">
         <v>45643.503680578702</v>
       </c>
-      <c r="B7" s="30"/>
+      <c r="B7" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C7" s="30" t="s">
         <v>19</v>
       </c>
@@ -1079,11 +1093,13 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>45683.669676157406</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1098,11 +1114,13 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>45657.471564467589</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1117,11 +1135,13 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>45657.37543388889</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1136,11 +1156,13 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>45656.78324715278</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1155,11 +1177,13 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="24">
         <v>45656.420678831018</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C12" s="28" t="s">
         <v>23</v>
       </c>
@@ -1174,11 +1198,13 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
         <v>45643.703139363424</v>
       </c>
-      <c r="B13" s="30"/>
+      <c r="B13" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C13" s="30" t="s">
         <v>23</v>
       </c>
@@ -1197,7 +1223,9 @@
       <c r="A14" s="6">
         <v>45680.791506851849</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
@@ -1216,7 +1244,9 @@
       <c r="A15" s="10">
         <v>45674.643437881939</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C15" s="11" t="s">
         <v>23</v>
       </c>
@@ -1235,7 +1265,9 @@
       <c r="A16" s="6">
         <v>45674.511061550926</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C16" s="7" t="s">
         <v>19</v>
       </c>
@@ -1254,7 +1286,9 @@
       <c r="A17" s="10">
         <v>45674.473131956023</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C17" s="11" t="s">
         <v>9</v>
       </c>
@@ -1273,7 +1307,9 @@
       <c r="A18" s="33">
         <v>45673.820017905091</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C18" s="34" t="s">
         <v>23</v>
       </c>
@@ -1292,7 +1328,9 @@
       <c r="A19" s="10">
         <v>45672.570346689812</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C19" s="11" t="s">
         <v>15</v>
       </c>
@@ -1307,17 +1345,19 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" ht="26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="26" x14ac:dyDescent="0.3">
       <c r="A20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="44"/>
+      <c r="B20" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C20" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
       <c r="H20" s="44"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -1330,13 +1370,15 @@
       <c r="A21" s="43">
         <v>45673.784612152776</v>
       </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49" t="s">
+      <c r="B21" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="49"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="48"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -1348,25 +1390,29 @@
       <c r="A22" s="43">
         <v>45683.444610949075</v>
       </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49" t="s">
+      <c r="B22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="49"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="40">
         <v>45679.456006030094</v>
       </c>
-      <c r="B23" s="46"/>
+      <c r="B23" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C23" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
       <c r="H23" s="46"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -1379,14 +1425,16 @@
       <c r="A24" s="43">
         <v>45674.816555115744</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49" t="s">
+      <c r="B24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="49"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="48"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -1394,11 +1442,13 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="25">
         <v>45656.896713599534</v>
       </c>
-      <c r="B25" s="29"/>
+      <c r="B25" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C25" s="29" t="s">
         <v>21</v>
       </c>
@@ -1414,11 +1464,13 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="37">
         <v>45653.78144575232</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C26" s="29" t="s">
         <v>21</v>
       </c>
@@ -1434,11 +1486,13 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="37">
         <v>45652.646530729166</v>
       </c>
-      <c r="B27" s="5"/>
+      <c r="B27" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C27" s="29" t="s">
         <v>21</v>
       </c>
@@ -1454,11 +1508,13 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="25">
         <v>45683.697622499996</v>
       </c>
-      <c r="B28" s="29"/>
+      <c r="B28" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C28" s="29" t="s">
         <v>21</v>
       </c>
@@ -1474,11 +1530,13 @@
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="25">
         <v>45683.650232222222</v>
       </c>
-      <c r="B29" s="29"/>
+      <c r="B29" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C29" s="29" t="s">
         <v>18</v>
       </c>
@@ -1494,11 +1552,13 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="25">
         <v>45683.585290312505</v>
       </c>
-      <c r="B30" s="29"/>
+      <c r="B30" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C30" s="29" t="s">
         <v>15</v>
       </c>
@@ -1514,11 +1574,13 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="25">
         <v>45683.498902361112</v>
       </c>
-      <c r="B31" s="29"/>
+      <c r="B31" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C31" s="29" t="s">
         <v>18</v>
       </c>
@@ -1534,11 +1596,13 @@
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="25">
         <v>45682.950552800925</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B32" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C32" s="29" t="s">
         <v>18</v>
       </c>
@@ -1554,11 +1618,13 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="25">
         <v>45681.022032291672</v>
       </c>
-      <c r="B33" s="29"/>
+      <c r="B33" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C33" s="29" t="s">
         <v>18</v>
       </c>
@@ -1578,7 +1644,9 @@
       <c r="A34" s="18">
         <v>45679.566921377314</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C34" s="2" t="s">
         <v>18</v>
       </c>
@@ -1598,7 +1666,9 @@
       <c r="A35" s="19">
         <v>45679.046571817133</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C35" s="3" t="s">
         <v>2</v>
       </c>
@@ -1618,7 +1688,9 @@
       <c r="A36" s="18">
         <v>45662.502799074078</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C36" s="2" t="s">
         <v>19</v>
       </c>
@@ -1634,11 +1706,13 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="19">
         <v>45656.962587812501</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C37" s="3" t="s">
         <v>18</v>
       </c>
@@ -1658,7 +1732,9 @@
       <c r="A38" s="18">
         <v>45656.711076041669</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C38" s="2" t="s">
         <v>23</v>
       </c>
@@ -1678,7 +1754,9 @@
       <c r="A39" s="19">
         <v>45656.708209317134</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C39" s="3" t="s">
         <v>23</v>
       </c>
@@ -1698,13 +1776,15 @@
       <c r="A40" s="24">
         <v>45653.935287280096</v>
       </c>
-      <c r="B40" s="28"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
+      <c r="B40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="51"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
       <c r="I40" s="7"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -1716,7 +1796,9 @@
       <c r="A41" s="26">
         <v>45653.873625717591</v>
       </c>
-      <c r="B41" s="30"/>
+      <c r="B41" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C41" s="30" t="s">
         <v>18</v>
       </c>
@@ -1736,7 +1818,9 @@
       <c r="A42" s="24">
         <v>45653.58239299769</v>
       </c>
-      <c r="B42" s="28"/>
+      <c r="B42" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C42" s="28" t="s">
         <v>15</v>
       </c>
@@ -1756,7 +1840,9 @@
       <c r="A43" s="26">
         <v>45652.684707453707</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C43" s="30" t="s">
         <v>18</v>
       </c>
@@ -1776,7 +1862,9 @@
       <c r="A44" s="24">
         <v>45652.678299039355</v>
       </c>
-      <c r="B44" s="28"/>
+      <c r="B44" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C44" s="28"/>
       <c r="D44" s="28"/>
       <c r="E44" s="28"/>
@@ -1794,7 +1882,9 @@
       <c r="A45" s="26">
         <v>45652.65138815972</v>
       </c>
-      <c r="B45" s="30"/>
+      <c r="B45" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C45" s="30" t="s">
         <v>18</v>
       </c>
@@ -1814,7 +1904,9 @@
       <c r="A46" s="24">
         <v>45646.574632615739</v>
       </c>
-      <c r="B46" s="28"/>
+      <c r="B46" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C46" s="28" t="s">
         <v>15</v>
       </c>
@@ -1834,7 +1926,9 @@
       <c r="A47" s="26">
         <v>45641.473255671299</v>
       </c>
-      <c r="B47" s="30"/>
+      <c r="B47" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C47" s="30" t="s">
         <v>3</v>
       </c>
@@ -1854,7 +1948,9 @@
       <c r="A48" s="33">
         <v>45683.429330462968</v>
       </c>
-      <c r="B48" s="34"/>
+      <c r="B48" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C48" s="34" t="s">
         <v>18</v>
       </c>
@@ -1874,7 +1970,9 @@
       <c r="A49" s="27">
         <v>45683.378273113427</v>
       </c>
-      <c r="B49" s="31"/>
+      <c r="B49" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C49" s="31" t="s">
         <v>18</v>
       </c>
@@ -1894,7 +1992,9 @@
       <c r="A50" s="33">
         <v>45682.776988506943</v>
       </c>
-      <c r="B50" s="34"/>
+      <c r="B50" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C50" s="36"/>
       <c r="D50" s="36"/>
       <c r="E50" s="36"/>
@@ -1912,7 +2012,9 @@
       <c r="A51" s="10">
         <v>45681.468215046298</v>
       </c>
-      <c r="B51" s="11"/>
+      <c r="B51" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C51" s="11" t="s">
         <v>18</v>
       </c>
@@ -1932,7 +2034,9 @@
       <c r="A52" s="6">
         <v>45681.418668217593</v>
       </c>
-      <c r="B52" s="7"/>
+      <c r="B52" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C52" s="7" t="s">
         <v>18</v>
       </c>
@@ -1952,7 +2056,9 @@
       <c r="A53" s="10">
         <v>45680.811210057873</v>
       </c>
-      <c r="B53" s="11"/>
+      <c r="B53" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C53" s="11" t="s">
         <v>18</v>
       </c>
@@ -1972,7 +2078,9 @@
       <c r="A54" s="33">
         <v>45680.552972430552</v>
       </c>
-      <c r="B54" s="34"/>
+      <c r="B54" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C54" s="34" t="s">
         <v>18</v>
       </c>
@@ -1992,7 +2100,9 @@
       <c r="A55" s="27">
         <v>45680.417232743057</v>
       </c>
-      <c r="B55" s="31"/>
+      <c r="B55" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C55" s="31" t="s">
         <v>23</v>
       </c>
@@ -2012,7 +2122,9 @@
       <c r="A56" s="33">
         <v>45680.037396215281</v>
       </c>
-      <c r="B56" s="34"/>
+      <c r="B56" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C56" s="34" t="s">
         <v>17</v>
       </c>
@@ -2032,7 +2144,9 @@
       <c r="A57" s="27">
         <v>45679.695603738423</v>
       </c>
-      <c r="B57" s="31"/>
+      <c r="B57" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C57" s="31" t="s">
         <v>19</v>
       </c>
@@ -2052,7 +2166,9 @@
       <c r="A58" s="6">
         <v>45677.41623101852</v>
       </c>
-      <c r="B58" s="7"/>
+      <c r="B58" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C58" s="7" t="s">
         <v>18</v>
       </c>
@@ -2072,7 +2188,9 @@
       <c r="A59" s="10">
         <v>45675.420260486106</v>
       </c>
-      <c r="B59" s="11"/>
+      <c r="B59" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C59" s="11" t="s">
         <v>5</v>
       </c>
@@ -2092,7 +2210,9 @@
       <c r="A60" s="33">
         <v>45674.669514398149</v>
       </c>
-      <c r="B60" s="34"/>
+      <c r="B60" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C60" s="34" t="s">
         <v>18</v>
       </c>
@@ -2112,7 +2232,9 @@
       <c r="A61" s="27">
         <v>45674.665730949069</v>
       </c>
-      <c r="B61" s="31"/>
+      <c r="B61" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C61" s="31" t="s">
         <v>18</v>
       </c>
@@ -2132,7 +2254,9 @@
       <c r="A62" s="6">
         <v>45674.574513564818</v>
       </c>
-      <c r="B62" s="7"/>
+      <c r="B62" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C62" s="7" t="s">
         <v>18</v>
       </c>
@@ -2152,7 +2276,9 @@
       <c r="A63" s="10">
         <v>45674.569825798608</v>
       </c>
-      <c r="B63" s="11"/>
+      <c r="B63" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C63" s="11" t="s">
         <v>18</v>
       </c>
@@ -2172,7 +2298,9 @@
       <c r="A64" s="33">
         <v>45674.494928831016</v>
       </c>
-      <c r="B64" s="34"/>
+      <c r="B64" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C64" s="34" t="s">
         <v>18</v>
       </c>
@@ -2192,7 +2320,9 @@
       <c r="A65" s="27">
         <v>45674.494073541668</v>
       </c>
-      <c r="B65" s="31"/>
+      <c r="B65" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C65" s="31" t="s">
         <v>18</v>
       </c>
@@ -2212,7 +2342,9 @@
       <c r="A66" s="6">
         <v>45674.436598483793</v>
       </c>
-      <c r="B66" s="7"/>
+      <c r="B66" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C66" s="7" t="s">
         <v>15</v>
       </c>
@@ -2232,7 +2364,9 @@
       <c r="A67" s="10">
         <v>45674.383986562505</v>
       </c>
-      <c r="B67" s="11"/>
+      <c r="B67" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C67" s="11" t="s">
         <v>18</v>
       </c>
@@ -2252,7 +2386,9 @@
       <c r="A68" s="6">
         <v>45674.37404299769</v>
       </c>
-      <c r="B68" s="7"/>
+      <c r="B68" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C68" s="7" t="s">
         <v>18</v>
       </c>
@@ -2272,7 +2408,9 @@
       <c r="A69" s="10">
         <v>45674.372054988431</v>
       </c>
-      <c r="B69" s="11"/>
+      <c r="B69" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C69" s="11" t="s">
         <v>23</v>
       </c>
@@ -2292,7 +2430,9 @@
       <c r="A70" s="6">
         <v>45674.353460798608</v>
       </c>
-      <c r="B70" s="7"/>
+      <c r="B70" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C70" s="7" t="s">
         <v>18</v>
       </c>
@@ -2312,7 +2452,9 @@
       <c r="A71" s="10">
         <v>45673.928360497681</v>
       </c>
-      <c r="B71" s="11"/>
+      <c r="B71" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C71" s="11" t="s">
         <v>18</v>
       </c>
@@ -2332,7 +2474,9 @@
       <c r="A72" s="33">
         <v>45673.780818449071</v>
       </c>
-      <c r="B72" s="34"/>
+      <c r="B72" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C72" s="34" t="s">
         <v>23</v>
       </c>
@@ -2352,13 +2496,15 @@
       <c r="A73" s="27">
         <v>45673.689383333331</v>
       </c>
-      <c r="B73" s="31"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
-      <c r="E73" s="51"/>
-      <c r="F73" s="51"/>
-      <c r="G73" s="51"/>
-      <c r="H73" s="51"/>
+      <c r="B73" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" s="50"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="50"/>
+      <c r="G73" s="50"/>
+      <c r="H73" s="50"/>
       <c r="I73" s="11"/>
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
@@ -2370,7 +2516,9 @@
       <c r="A74" s="33">
         <v>45673.674294942131</v>
       </c>
-      <c r="B74" s="34"/>
+      <c r="B74" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C74" s="34" t="s">
         <v>18</v>
       </c>
@@ -2390,7 +2538,9 @@
       <c r="A75" s="27">
         <v>45673.674258090279</v>
       </c>
-      <c r="B75" s="31"/>
+      <c r="B75" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C75" s="31" t="s">
         <v>18</v>
       </c>
@@ -2410,7 +2560,9 @@
       <c r="A76" s="33">
         <v>45673.643358333335</v>
       </c>
-      <c r="B76" s="34"/>
+      <c r="B76" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C76" s="34" t="s">
         <v>18</v>
       </c>
@@ -2430,7 +2582,9 @@
       <c r="A77" s="27">
         <v>45672.851519074073</v>
       </c>
-      <c r="B77" s="31"/>
+      <c r="B77" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C77" s="31" t="s">
         <v>15</v>
       </c>
@@ -2450,7 +2604,9 @@
       <c r="A78" s="33">
         <v>45672.798996840276</v>
       </c>
-      <c r="B78" s="34"/>
+      <c r="B78" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C78" s="34" t="s">
         <v>18</v>
       </c>
@@ -2470,7 +2626,9 @@
       <c r="A79" s="27">
         <v>45672.725427187499</v>
       </c>
-      <c r="B79" s="31"/>
+      <c r="B79" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C79" s="31" t="s">
         <v>19</v>
       </c>
@@ -2490,7 +2648,9 @@
       <c r="A80" s="6">
         <v>45672.555116782409</v>
       </c>
-      <c r="B80" s="7"/>
+      <c r="B80" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C80" s="7" t="s">
         <v>18</v>
       </c>
@@ -2510,7 +2670,9 @@
       <c r="A81" s="10">
         <v>45672.531103946763</v>
       </c>
-      <c r="B81" s="11"/>
+      <c r="B81" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C81" s="11" t="s">
         <v>15</v>
       </c>
@@ -2530,7 +2692,9 @@
       <c r="A82" s="6">
         <v>45672.505838020836</v>
       </c>
-      <c r="B82" s="7"/>
+      <c r="B82" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C82" s="7" t="s">
         <v>18</v>
       </c>
@@ -2550,7 +2714,9 @@
       <c r="A83" s="10">
         <v>45672.496103518519</v>
       </c>
-      <c r="B83" s="11"/>
+      <c r="B83" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C83" s="11" t="s">
         <v>18</v>
       </c>
@@ -2570,7 +2736,9 @@
       <c r="A84" s="6">
         <v>45672.449038715276</v>
       </c>
-      <c r="B84" s="7"/>
+      <c r="B84" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C84" s="7" t="s">
         <v>18</v>
       </c>
@@ -2590,7 +2758,9 @@
       <c r="A85" s="10">
         <v>45672.446658506946</v>
       </c>
-      <c r="B85" s="11"/>
+      <c r="B85" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C85" s="11" t="s">
         <v>18</v>
       </c>
@@ -2610,13 +2780,15 @@
       <c r="A86" s="42">
         <v>45672.357569398147</v>
       </c>
-      <c r="B86" s="48"/>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
-      <c r="E86" s="50"/>
-      <c r="F86" s="50"/>
-      <c r="G86" s="50"/>
-      <c r="H86" s="50"/>
+      <c r="B86" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" s="49"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="49"/>
+      <c r="F86" s="49"/>
+      <c r="G86" s="49"/>
+      <c r="H86" s="49"/>
       <c r="I86" s="14"/>
       <c r="J86" s="15"/>
       <c r="K86" s="15"/>
@@ -2628,14 +2800,16 @@
       <c r="A87" s="41">
         <v>45683.566615509262</v>
       </c>
-      <c r="B87" s="47"/>
+      <c r="B87" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C87" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D87" s="55"/>
-      <c r="E87" s="55"/>
-      <c r="F87" s="55"/>
-      <c r="G87" s="55"/>
+      <c r="D87" s="54"/>
+      <c r="E87" s="54"/>
+      <c r="F87" s="54"/>
+      <c r="G87" s="54"/>
       <c r="H87" s="47"/>
       <c r="I87" s="16"/>
       <c r="J87" s="17"/>
@@ -2648,14 +2822,16 @@
       <c r="A88" s="40">
         <v>45683.717176782404</v>
       </c>
-      <c r="B88" s="46"/>
+      <c r="B88" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C88" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D88" s="54"/>
-      <c r="E88" s="54"/>
-      <c r="F88" s="54"/>
-      <c r="G88" s="54"/>
+      <c r="D88" s="53"/>
+      <c r="E88" s="53"/>
+      <c r="F88" s="53"/>
+      <c r="G88" s="53"/>
       <c r="H88" s="46"/>
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
@@ -2664,11 +2840,13 @@
       <c r="M88" s="5"/>
       <c r="N88" s="5"/>
     </row>
-    <row r="89" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="39">
         <v>45683.714303020832</v>
       </c>
-      <c r="B89" s="45"/>
+      <c r="B89" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C89" s="45" t="s">
         <v>21</v>
       </c>
@@ -2685,170 +2863,226 @@
       <c r="N89" s="21"/>
     </row>
     <row r="90" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="B90" s="7"/>
+      <c r="B90" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C90" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="B91" s="31"/>
+      <c r="B91" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C91" s="32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B92" s="2"/>
+    <row r="92" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="B92" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C92" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="B93" s="31"/>
+      <c r="B93" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C93" s="32" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="B94" s="7"/>
+      <c r="B94" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C94" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="B95" s="7"/>
+      <c r="B95" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C95" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="B96" s="31"/>
+      <c r="B96" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C96" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="97" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B97" s="7"/>
+      <c r="B97" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C97" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="3"/>
+    <row r="98" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B98" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C98" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="2"/>
+    <row r="99" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B99" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C99" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="30"/>
+    <row r="100" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B100" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C100" s="30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="2"/>
+    <row r="101" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B101" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C101" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="3"/>
+    <row r="102" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B102" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C102" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="2"/>
+    <row r="103" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B103" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C103" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="3"/>
+    <row r="104" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B104" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C104" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="28"/>
+    <row r="105" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B105" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C105" s="28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="30"/>
+    <row r="106" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B106" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C106" s="30" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="107" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B107" s="7"/>
+      <c r="B107" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C107" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="108" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B108" s="11"/>
+      <c r="B108" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C108" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B109" s="7"/>
+      <c r="B109" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C109" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B110" s="11"/>
+      <c r="B110" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C110" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B111" s="34"/>
+      <c r="B111" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="C111" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B112" s="11"/>
+      <c r="B112" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C112" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="2:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="B113" s="44"/>
-      <c r="C113" s="53" t="s">
+    <row r="113" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="B113" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C113" s="52" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="114" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B114" s="49"/>
-      <c r="C114" s="56" t="s">
+      <c r="B114" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C114" s="55" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="115" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B115" s="49"/>
-      <c r="C115" s="56" t="s">
+      <c r="B115" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C115" s="55" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="116" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B116" s="46"/>
-      <c r="C116" s="54" t="s">
+      <c r="B116" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" s="53" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="117" spans="2:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="B117" s="49"/>
-      <c r="C117" s="56" t="s">
+      <c r="B117" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C117" s="55" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>